<commit_message>
added input/output label and typeRef
</commit_message>
<xml_diff>
--- a/xlsx-dmn-converter/src/test/resources/test1.xlsx
+++ b/xlsx-dmn-converter/src/test/resources/test1.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\camunda\repos\other\camunda-dmn-xslx\xslx-dmn-converter\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\camundaBPM\src\PLAYGROUND\camunda-dmn-xlsx\xlsx-dmn-converter\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18636" windowHeight="6240"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18630" windowHeight="6240"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
   <si>
     <t>input1</t>
   </si>
@@ -47,10 +47,13 @@
     <t>&lt;= 10</t>
   </si>
   <si>
-    <t>foofoo</t>
-  </si>
-  <si>
     <t>barbar</t>
+  </si>
+  <si>
+    <t>xxx</t>
+  </si>
+  <si>
+    <t>One Result</t>
   </si>
 </sst>
 </file>
@@ -371,12 +374,12 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -387,7 +390,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -395,10 +398,10 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -406,10 +409,10 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -417,10 +420,10 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>

</xml_diff>